<commit_message>
I debug FitPDT.cpp && extract the WMUdata.
</commit_message>
<xml_diff>
--- a/12KinematicLineProjection/ProtonRecoilRunsForCalibrationsCopy.xlsx
+++ b/12KinematicLineProjection/ProtonRecoilRunsForCalibrationsCopy.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
   <si>
     <t>Run Number</t>
   </si>
@@ -57,6 +56,9 @@
   </si>
   <si>
     <t>….</t>
+  </si>
+  <si>
+    <t>This dataset is really bad!!</t>
   </si>
 </sst>
 </file>
@@ -157,12 +159,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -175,6 +171,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -482,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -498,27 +500,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -547,356 +549,356 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>4589</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
         <v>56.6</v>
       </c>
-      <c r="D4" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E4" s="7">
-        <v>170</v>
-      </c>
-      <c r="F4" s="5">
-        <v>200</v>
-      </c>
-      <c r="G4" s="5">
-        <v>200</v>
-      </c>
-      <c r="H4" s="5"/>
+      <c r="D4" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E4" s="5">
+        <v>170</v>
+      </c>
+      <c r="F4" s="3">
+        <v>200</v>
+      </c>
+      <c r="G4" s="3">
+        <v>200</v>
+      </c>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="3">
         <v>4588</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
         <v>56.6</v>
       </c>
-      <c r="D5" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E5" s="7">
-        <v>170</v>
-      </c>
-      <c r="F5" s="5">
-        <v>200</v>
-      </c>
-      <c r="G5" s="5">
-        <v>200</v>
-      </c>
-      <c r="H5" s="5"/>
+      <c r="D5" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>170</v>
+      </c>
+      <c r="F5" s="3">
+        <v>200</v>
+      </c>
+      <c r="G5" s="3">
+        <v>200</v>
+      </c>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="3">
         <v>4587</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3">
         <v>56.6</v>
       </c>
-      <c r="D6" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E6" s="7">
-        <v>170</v>
-      </c>
-      <c r="F6" s="5">
-        <v>200</v>
-      </c>
-      <c r="G6" s="5">
-        <v>200</v>
-      </c>
-      <c r="H6" s="5"/>
+      <c r="D6" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>170</v>
+      </c>
+      <c r="F6" s="3">
+        <v>200</v>
+      </c>
+      <c r="G6" s="3">
+        <v>200</v>
+      </c>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="3">
         <v>4586</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3">
         <v>56.6</v>
       </c>
-      <c r="D7" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E7" s="7">
-        <v>170</v>
-      </c>
-      <c r="F7" s="5">
-        <v>200</v>
-      </c>
-      <c r="G7" s="5">
-        <v>200</v>
-      </c>
-      <c r="H7" s="5"/>
+      <c r="D7" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>170</v>
+      </c>
+      <c r="F7" s="3">
+        <v>200</v>
+      </c>
+      <c r="G7" s="3">
+        <v>200</v>
+      </c>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="3">
         <v>4585</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3">
         <v>56.6</v>
       </c>
-      <c r="D8" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E8" s="7">
-        <v>170</v>
-      </c>
-      <c r="F8" s="5">
-        <v>200</v>
-      </c>
-      <c r="G8" s="5">
-        <v>200</v>
-      </c>
-      <c r="H8" s="5">
+      <c r="D8" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E8" s="5">
+        <v>170</v>
+      </c>
+      <c r="F8" s="3">
+        <v>200</v>
+      </c>
+      <c r="G8" s="3">
+        <v>200</v>
+      </c>
+      <c r="H8" s="3">
         <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="3">
         <v>4584</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3">
         <v>28</v>
       </c>
-      <c r="D10" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E10" s="7">
-        <v>170</v>
-      </c>
-      <c r="F10" s="5">
-        <v>200</v>
-      </c>
-      <c r="G10" s="5">
-        <v>200</v>
-      </c>
-      <c r="H10" s="5"/>
+      <c r="D10" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E10" s="5">
+        <v>170</v>
+      </c>
+      <c r="F10" s="3">
+        <v>200</v>
+      </c>
+      <c r="G10" s="3">
+        <v>200</v>
+      </c>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="3">
         <v>4583</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3">
         <v>28</v>
       </c>
-      <c r="D11" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E11" s="7">
-        <v>170</v>
-      </c>
-      <c r="F11" s="5">
-        <v>200</v>
-      </c>
-      <c r="G11" s="5">
-        <v>200</v>
-      </c>
-      <c r="H11" s="5"/>
+      <c r="D11" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E11" s="5">
+        <v>170</v>
+      </c>
+      <c r="F11" s="3">
+        <v>200</v>
+      </c>
+      <c r="G11" s="3">
+        <v>200</v>
+      </c>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="3">
         <v>4582</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3">
         <v>28</v>
       </c>
-      <c r="D12" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E12" s="7">
-        <v>170</v>
-      </c>
-      <c r="F12" s="5">
-        <v>200</v>
-      </c>
-      <c r="G12" s="5">
-        <v>200</v>
-      </c>
-      <c r="H12" s="5"/>
+      <c r="D12" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E12" s="5">
+        <v>170</v>
+      </c>
+      <c r="F12" s="3">
+        <v>200</v>
+      </c>
+      <c r="G12" s="3">
+        <v>200</v>
+      </c>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="3">
         <v>4581</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3">
         <v>28</v>
       </c>
-      <c r="D13" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E13" s="7">
-        <v>170</v>
-      </c>
-      <c r="F13" s="5">
-        <v>200</v>
-      </c>
-      <c r="G13" s="5">
-        <v>200</v>
-      </c>
-      <c r="H13" s="5"/>
+      <c r="D13" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E13" s="5">
+        <v>170</v>
+      </c>
+      <c r="F13" s="3">
+        <v>200</v>
+      </c>
+      <c r="G13" s="3">
+        <v>200</v>
+      </c>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="3">
         <v>4580</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3">
         <v>28</v>
       </c>
-      <c r="D14" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E14" s="7">
-        <v>170</v>
-      </c>
-      <c r="F14" s="5">
-        <v>200</v>
-      </c>
-      <c r="G14" s="5">
-        <v>200</v>
-      </c>
-      <c r="H14" s="5"/>
+      <c r="D14" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E14" s="5">
+        <v>170</v>
+      </c>
+      <c r="F14" s="3">
+        <v>200</v>
+      </c>
+      <c r="G14" s="3">
+        <v>200</v>
+      </c>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="3">
         <v>4579</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3">
         <v>28</v>
       </c>
-      <c r="D15" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E15" s="7">
-        <v>170</v>
-      </c>
-      <c r="F15" s="5">
-        <v>200</v>
-      </c>
-      <c r="G15" s="5">
-        <v>200</v>
-      </c>
-      <c r="H15" s="5"/>
+      <c r="D15" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E15" s="5">
+        <v>170</v>
+      </c>
+      <c r="F15" s="3">
+        <v>200</v>
+      </c>
+      <c r="G15" s="3">
+        <v>200</v>
+      </c>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="3">
         <v>4578</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3">
         <v>28</v>
       </c>
-      <c r="D16" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E16" s="7">
-        <v>170</v>
-      </c>
-      <c r="F16" s="5">
-        <v>200</v>
-      </c>
-      <c r="G16" s="5">
-        <v>200</v>
-      </c>
-      <c r="H16" s="5"/>
+      <c r="D16" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E16" s="5">
+        <v>170</v>
+      </c>
+      <c r="F16" s="3">
+        <v>200</v>
+      </c>
+      <c r="G16" s="3">
+        <v>200</v>
+      </c>
+      <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="3">
         <v>4577</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="B17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="3">
         <v>28</v>
       </c>
-      <c r="D17" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E17" s="7">
-        <v>170</v>
-      </c>
-      <c r="F17" s="5">
-        <v>200</v>
-      </c>
-      <c r="G17" s="5">
-        <v>200</v>
-      </c>
-      <c r="H17" s="5">
+      <c r="D17" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E17" s="5">
+        <v>170</v>
+      </c>
+      <c r="F17" s="3">
+        <v>200</v>
+      </c>
+      <c r="G17" s="3">
+        <v>200</v>
+      </c>
+      <c r="H17" s="3">
         <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
+      <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="3">
         <v>4332</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="5">
+      <c r="B19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="3">
         <v>56.6</v>
       </c>
-      <c r="D19" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E19" s="7">
-        <v>170</v>
-      </c>
-      <c r="F19" s="5">
-        <v>200</v>
-      </c>
-      <c r="G19" s="5">
-        <v>200</v>
-      </c>
-      <c r="H19" s="5"/>
+      <c r="D19" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E19" s="5">
+        <v>170</v>
+      </c>
+      <c r="F19" s="3">
+        <v>200</v>
+      </c>
+      <c r="G19" s="3">
+        <v>200</v>
+      </c>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4040</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C20">
@@ -916,7 +918,7 @@
       <c r="A21">
         <v>4039</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C21">
@@ -936,150 +938,150 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="3">
         <v>4037</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="5">
+      <c r="B23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="3">
         <v>28</v>
       </c>
-      <c r="D23" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E23" s="7">
-        <v>170</v>
-      </c>
-      <c r="F23" s="5">
-        <v>200</v>
-      </c>
-      <c r="G23" s="5">
-        <v>200</v>
-      </c>
-      <c r="H23" s="5"/>
+      <c r="D23" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E23" s="5">
+        <v>170</v>
+      </c>
+      <c r="F23" s="3">
+        <v>200</v>
+      </c>
+      <c r="G23" s="3">
+        <v>200</v>
+      </c>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="3">
         <v>4036</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="5">
+      <c r="B24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="3">
         <v>28</v>
       </c>
-      <c r="D24" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E24" s="7">
-        <v>170</v>
-      </c>
-      <c r="F24" s="5">
-        <v>200</v>
-      </c>
-      <c r="G24" s="5">
-        <v>200</v>
-      </c>
-      <c r="H24" s="5"/>
+      <c r="D24" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E24" s="5">
+        <v>170</v>
+      </c>
+      <c r="F24" s="3">
+        <v>200</v>
+      </c>
+      <c r="G24" s="3">
+        <v>200</v>
+      </c>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="3">
         <v>4035</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="5">
+      <c r="B25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="3">
         <v>28</v>
       </c>
-      <c r="D25" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E25" s="7">
-        <v>170</v>
-      </c>
-      <c r="F25" s="5">
-        <v>200</v>
-      </c>
-      <c r="G25" s="5">
-        <v>200</v>
-      </c>
-      <c r="H25" s="5"/>
+      <c r="D25" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E25" s="5">
+        <v>170</v>
+      </c>
+      <c r="F25" s="3">
+        <v>200</v>
+      </c>
+      <c r="G25" s="3">
+        <v>200</v>
+      </c>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="3">
         <v>4034</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="5">
+      <c r="B26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="3">
         <v>28</v>
       </c>
-      <c r="D26" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E26" s="7">
-        <v>170</v>
-      </c>
-      <c r="F26" s="5">
-        <v>200</v>
-      </c>
-      <c r="G26" s="5">
-        <v>200</v>
-      </c>
-      <c r="H26" s="5">
+      <c r="D26" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E26" s="5">
+        <v>170</v>
+      </c>
+      <c r="F26" s="3">
+        <v>200</v>
+      </c>
+      <c r="G26" s="3">
+        <v>200</v>
+      </c>
+      <c r="H26" s="3">
         <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="3">
         <v>4022</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="5">
+      <c r="B28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="3">
         <v>139.80000000000001</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="8">
         <v>2E-3</v>
       </c>
-      <c r="E28" s="7">
-        <v>170</v>
-      </c>
-      <c r="F28" s="5">
-        <v>200</v>
-      </c>
-      <c r="G28" s="5">
-        <v>200</v>
-      </c>
-      <c r="H28" s="5"/>
+      <c r="E28" s="5">
+        <v>170</v>
+      </c>
+      <c r="F28" s="3">
+        <v>200</v>
+      </c>
+      <c r="G28" s="3">
+        <v>200</v>
+      </c>
+      <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="3">
         <v>4021</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="5">
+      <c r="B29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="3">
         <v>139.80000000000001</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="8">
         <v>2E-3</v>
       </c>
-      <c r="E29" s="7">
-        <v>170</v>
-      </c>
-      <c r="F29" s="5">
-        <v>200</v>
-      </c>
-      <c r="G29" s="5">
-        <v>200</v>
-      </c>
-      <c r="H29" s="5">
+      <c r="E29" s="5">
+        <v>170</v>
+      </c>
+      <c r="F29" s="3">
+        <v>200</v>
+      </c>
+      <c r="G29" s="3">
+        <v>200</v>
+      </c>
+      <c r="H29" s="3">
         <v>70</v>
       </c>
     </row>
@@ -1087,13 +1089,13 @@
       <c r="A31">
         <v>4005</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C31">
         <v>139.80000000000001</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="9">
         <v>2E-3</v>
       </c>
       <c r="E31">
@@ -1110,13 +1112,13 @@
       <c r="A32">
         <v>4004</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C32">
         <v>139.80000000000001</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="9">
         <v>2E-3</v>
       </c>
       <c r="E32">
@@ -1133,13 +1135,13 @@
       <c r="A33">
         <v>4003</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C33">
         <v>139.80000000000001</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="9">
         <v>2E-3</v>
       </c>
       <c r="E33">
@@ -1156,13 +1158,13 @@
       <c r="A34">
         <v>4002</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C34">
         <v>139.80000000000001</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="9">
         <v>2E-3</v>
       </c>
       <c r="E34">
@@ -1179,13 +1181,13 @@
       <c r="A35">
         <v>4001</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C35">
         <v>139.80000000000001</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="9">
         <v>2E-3</v>
       </c>
       <c r="E35">
@@ -1202,13 +1204,13 @@
       <c r="A36">
         <v>4000</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C36">
         <v>139.80000000000001</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="9">
         <v>2E-3</v>
       </c>
       <c r="E36">
@@ -1225,248 +1227,250 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+      <c r="A38" s="3">
         <v>2829</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="3">
         <v>139.80000000000001</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="8">
         <v>2E-3</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="6">
         <v>130</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="3">
         <v>130</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="3">
         <v>130</v>
       </c>
-      <c r="H38" s="5"/>
+      <c r="H38" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+      <c r="A39" s="3">
         <v>2828</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="3">
         <v>139.80000000000001</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D39" s="8">
         <v>2E-3</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="6">
         <v>130</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F39" s="3">
         <v>130</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="3">
         <v>130</v>
       </c>
-      <c r="H39" s="5"/>
+      <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+      <c r="A40" s="3">
         <v>2827</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="3">
         <v>139.80000000000001</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="8">
         <v>2E-3</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E40" s="6">
         <v>130</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="3">
         <v>130</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="3">
         <v>130</v>
       </c>
-      <c r="H40" s="5"/>
+      <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+      <c r="A41" s="3">
         <v>2826</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="3">
         <v>139.80000000000001</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D41" s="8">
         <v>2E-3</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="6">
         <v>130</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="3">
         <v>130</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="3">
         <v>130</v>
       </c>
-      <c r="H41" s="5"/>
+      <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+      <c r="A42" s="3">
         <v>2825</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="3">
         <v>139.80000000000001</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="8">
         <v>2E-3</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="6">
         <v>130</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="3">
         <v>130</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="3">
         <v>130</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H42" s="3">
         <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
+      <c r="A44" s="3">
         <v>2312</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="3">
         <v>56.6</v>
       </c>
-      <c r="D44" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E44" s="7">
-        <v>170</v>
-      </c>
-      <c r="F44" s="5">
-        <v>200</v>
-      </c>
-      <c r="G44" s="5">
-        <v>200</v>
-      </c>
-      <c r="H44" s="5">
+      <c r="D44" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E44" s="5">
+        <v>170</v>
+      </c>
+      <c r="F44" s="3">
+        <v>200</v>
+      </c>
+      <c r="G44" s="3">
+        <v>200</v>
+      </c>
+      <c r="H44" s="3">
         <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
+      <c r="A47" s="3">
         <v>2037</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="3">
         <v>39</v>
       </c>
-      <c r="D47" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E47" s="9">
-        <v>200</v>
-      </c>
-      <c r="F47" s="5">
-        <v>200</v>
-      </c>
-      <c r="G47" s="5">
-        <v>200</v>
-      </c>
-      <c r="H47" s="5"/>
+      <c r="D47" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E47" s="7">
+        <v>200</v>
+      </c>
+      <c r="F47" s="3">
+        <v>200</v>
+      </c>
+      <c r="G47" s="3">
+        <v>200</v>
+      </c>
+      <c r="H47" s="3"/>
     </row>
     <row r="48" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
+      <c r="A48" s="3">
         <v>2036</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="3">
         <v>39</v>
       </c>
-      <c r="D48" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E48" s="9">
-        <v>200</v>
-      </c>
-      <c r="F48" s="5">
-        <v>200</v>
-      </c>
-      <c r="G48" s="5">
-        <v>200</v>
-      </c>
-      <c r="H48" s="5"/>
+      <c r="D48" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E48" s="7">
+        <v>200</v>
+      </c>
+      <c r="F48" s="3">
+        <v>200</v>
+      </c>
+      <c r="G48" s="3">
+        <v>200</v>
+      </c>
+      <c r="H48" s="3"/>
     </row>
     <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E49" s="9">
-        <v>200</v>
-      </c>
-      <c r="F49" s="5">
-        <v>200</v>
-      </c>
-      <c r="G49" s="5">
-        <v>200</v>
-      </c>
-      <c r="H49" s="5"/>
+      <c r="D49" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E49" s="7">
+        <v>200</v>
+      </c>
+      <c r="F49" s="3">
+        <v>200</v>
+      </c>
+      <c r="G49" s="3">
+        <v>200</v>
+      </c>
+      <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
+      <c r="A50" s="3">
         <v>2013</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="3">
         <v>39</v>
       </c>
-      <c r="D50" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E50" s="9">
-        <v>200</v>
-      </c>
-      <c r="F50" s="5">
-        <v>200</v>
-      </c>
-      <c r="G50" s="5">
-        <v>200</v>
-      </c>
-      <c r="H50" s="5"/>
+      <c r="D50" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E50" s="7">
+        <v>200</v>
+      </c>
+      <c r="F50" s="3">
+        <v>200</v>
+      </c>
+      <c r="G50" s="3">
+        <v>200</v>
+      </c>
+      <c r="H50" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>